<commit_message>
Added Dates in Gantt Chart
</commit_message>
<xml_diff>
--- a/Gantt-Chart.xlsx
+++ b/Gantt-Chart.xlsx
@@ -16,130 +16,130 @@
     <t>Task / Day</t>
   </si>
   <si>
-    <t>W1-D1</t>
-  </si>
-  <si>
-    <t>W1-D2</t>
-  </si>
-  <si>
-    <t>W1-D3</t>
-  </si>
-  <si>
-    <t>W1-D4</t>
-  </si>
-  <si>
-    <t>W1-D5</t>
-  </si>
-  <si>
-    <t>W1-D6</t>
-  </si>
-  <si>
-    <t>W1-D7</t>
-  </si>
-  <si>
-    <t>W2-D1</t>
-  </si>
-  <si>
-    <t>W2-D2</t>
-  </si>
-  <si>
-    <t>W2-D3</t>
-  </si>
-  <si>
-    <t>W2-D4</t>
-  </si>
-  <si>
-    <t>W2-D5</t>
-  </si>
-  <si>
-    <t>W2-D6</t>
-  </si>
-  <si>
-    <t>W2-D7</t>
-  </si>
-  <si>
-    <t>W3-D1</t>
-  </si>
-  <si>
-    <t>W3-D2</t>
-  </si>
-  <si>
-    <t>W3-D3</t>
-  </si>
-  <si>
-    <t>W3-D4</t>
-  </si>
-  <si>
-    <t>W3-D5</t>
-  </si>
-  <si>
-    <t>W3-D6</t>
-  </si>
-  <si>
-    <t>W3-D7</t>
-  </si>
-  <si>
-    <t>W4-D1</t>
-  </si>
-  <si>
-    <t>W4-D2</t>
-  </si>
-  <si>
-    <t>W4-D3</t>
-  </si>
-  <si>
-    <t>W4-D4</t>
-  </si>
-  <si>
-    <t>W4-D5</t>
-  </si>
-  <si>
-    <t>W4-D6</t>
-  </si>
-  <si>
-    <t>W4-D7</t>
-  </si>
-  <si>
-    <t>W5-D1</t>
-  </si>
-  <si>
-    <t>W5-D2</t>
-  </si>
-  <si>
-    <t>W5-D3</t>
-  </si>
-  <si>
-    <t>W5-D4</t>
-  </si>
-  <si>
-    <t>W5-D5</t>
-  </si>
-  <si>
-    <t>W5-D6</t>
-  </si>
-  <si>
-    <t>W5-D7</t>
-  </si>
-  <si>
-    <t>W6-D1</t>
-  </si>
-  <si>
-    <t>W6-D2</t>
-  </si>
-  <si>
-    <t>W6-D3</t>
-  </si>
-  <si>
-    <t>W6-D4</t>
-  </si>
-  <si>
-    <t>W6-D5</t>
-  </si>
-  <si>
-    <t>W6-D6</t>
-  </si>
-  <si>
-    <t>W6-D7</t>
+    <t>W1-D1(24/1)</t>
+  </si>
+  <si>
+    <t>W1-D2(26/1)</t>
+  </si>
+  <si>
+    <t>W1-D3(28/1)</t>
+  </si>
+  <si>
+    <t>W1-D4(30/1)</t>
+  </si>
+  <si>
+    <t>W1-D5(31/1)</t>
+  </si>
+  <si>
+    <t>W1-D6(3/2)</t>
+  </si>
+  <si>
+    <t>W1-D7(4/2)</t>
+  </si>
+  <si>
+    <t>W2-D1(6/2)</t>
+  </si>
+  <si>
+    <t>W2-D2(7/2)</t>
+  </si>
+  <si>
+    <t>W2-D3(11/2)</t>
+  </si>
+  <si>
+    <t>W2-D4(12/2)</t>
+  </si>
+  <si>
+    <t>W2-D5(13/2)</t>
+  </si>
+  <si>
+    <t>W2-D6(14/2)</t>
+  </si>
+  <si>
+    <t>W2-D7(16/2)</t>
+  </si>
+  <si>
+    <t>W3-D1(17/2)</t>
+  </si>
+  <si>
+    <t>W3-D2(18/2)</t>
+  </si>
+  <si>
+    <t>W3-D3(19/2)</t>
+  </si>
+  <si>
+    <t>W3-D4(20/2)</t>
+  </si>
+  <si>
+    <t>W3-D5(21/2)</t>
+  </si>
+  <si>
+    <t>W3-D6(23/2)</t>
+  </si>
+  <si>
+    <t>W3-D7(24/2)</t>
+  </si>
+  <si>
+    <t>W4-D1(25/2)</t>
+  </si>
+  <si>
+    <t>W4-D2(26/2)</t>
+  </si>
+  <si>
+    <t>W4-D3(27/2)</t>
+  </si>
+  <si>
+    <t>W4-D4(28/2)</t>
+  </si>
+  <si>
+    <t>W4-D5(2/3)</t>
+  </si>
+  <si>
+    <t>W4-D6(3/3)</t>
+  </si>
+  <si>
+    <t>W4-D7(4/3)</t>
+  </si>
+  <si>
+    <t>W5-D1(5/3)</t>
+  </si>
+  <si>
+    <t>W5-D2(6/3)</t>
+  </si>
+  <si>
+    <t>W5-D3(7/3)</t>
+  </si>
+  <si>
+    <t>W5-D4(9/3)</t>
+  </si>
+  <si>
+    <t>W5-D5(10/3)</t>
+  </si>
+  <si>
+    <t>W5-D6(11/3)</t>
+  </si>
+  <si>
+    <t>W5-D7(12/3)</t>
+  </si>
+  <si>
+    <t>W6-D1(13/3)</t>
+  </si>
+  <si>
+    <t>W6-D2(14/3)</t>
+  </si>
+  <si>
+    <t>W6-D3(16/3)</t>
+  </si>
+  <si>
+    <t>W6-D4(17/3)</t>
+  </si>
+  <si>
+    <t>W6-D5(18/3)</t>
+  </si>
+  <si>
+    <t>W6-D6(19/3)</t>
+  </si>
+  <si>
+    <t>W6-D7(20/3)</t>
   </si>
   <si>
     <t>Python Memory Model &amp; Internals</t>

</xml_diff>